<commit_message>
process run test planning completed.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/process_run_record_test_cases.xlsx
+++ b/soberano/test_cases/process_run_record_test_cases.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="inventory operation record test" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="process run record tests" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">user9</t>
   </si>
   <si>
-    <t xml:space="preserve">mmpr2</t>
+    <t xml:space="preserve">mpr2</t>
   </si>
   <si>
     <t xml:space="preserve">user17</t>
@@ -290,10 +290,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.45"/>

</xml_diff>